<commit_message>
add raw data to figures
</commit_message>
<xml_diff>
--- a/code_data_relationships.xlsx
+++ b/code_data_relationships.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AmyKendig/Dropbox (UFL)/big-oaks-field-experiment-2018-2019/microstegium-bipolaris/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB614095-188F-E84A-A777-BDD593DD5D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A97A12-3404-6E4B-81D7-71A438C89A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37880" yWindow="580" windowWidth="30760" windowHeight="28220" xr2:uid="{A8324B94-3DCB-F445-8C87-9FFCE272213B}"/>
+    <workbookView xWindow="42160" yWindow="500" windowWidth="26640" windowHeight="28220" xr2:uid="{A8324B94-3DCB-F445-8C87-9FFCE272213B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,12 +173,78 @@
         </r>
       </text>
     </comment>
+    <comment ref="E26" authorId="0" shapeId="0" xr:uid="{5EFFD713-1406-DD4F-9C99-5F013C00BA02}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E27" authorId="0" shapeId="0" xr:uid="{7004317B-090F-F845-9417-EE971B3D7469}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
   <si>
     <t>Code</t>
   </si>
@@ -403,38 +469,139 @@
   </si>
   <si>
     <t>Dependency source 2</t>
+  </si>
+  <si>
+    <t>disease_treatment_effects_2018_2019_density_exp.R</t>
+  </si>
+  <si>
+    <t>focal_severity_model_aug_2019_dens_exp.rda</t>
+  </si>
+  <si>
+    <t>sevD2Mod_sev_dens_aug</t>
+  </si>
+  <si>
+    <t>focal_severity_model_jul_2019_dens_exp.rda</t>
+  </si>
+  <si>
+    <t>sevD2Mod_sev_dens_jul</t>
+  </si>
+  <si>
+    <t>Figure 3,
+Figure S2-S4,
+Tables S10–S13 &amp; S24</t>
+  </si>
+  <si>
+    <t>ev_plot_biomass_seeds_density_2019_density_exp.R</t>
+  </si>
+  <si>
+    <t>Figure S6, 
+Tables S1-S2</t>
+  </si>
+  <si>
+    <t>bgBioD2Dat</t>
+  </si>
+  <si>
+    <t>evBioD2Dat</t>
+  </si>
+  <si>
+    <t>evSeedD2Dat</t>
+  </si>
+  <si>
+    <t>ev_processed_seeds_both_year_conversion_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>bg_processed_biomass_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>bg_biomass_data_processing_2019_density_exp.R</t>
+  </si>
+  <si>
+    <t>ev_biomass_seeds_oct_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_seeds_data_processing_2018.R</t>
+  </si>
+  <si>
+    <t>ev_seeds_data_processing_2019.R</t>
+  </si>
+  <si>
+    <t>sevD2Dat3_aug2</t>
+  </si>
+  <si>
+    <t>focal_severity_model_data_aug_2019_dens_exp.csv</t>
+  </si>
+  <si>
+    <t>sevD2Dat3_jul2</t>
+  </si>
+  <si>
+    <t>ocal_severity_model_data_jul_2019_dens_exp.csv</t>
+  </si>
+  <si>
+    <t>mvGermD1Mod3</t>
+  </si>
+  <si>
+    <t>mvGermD1Dat</t>
+  </si>
+  <si>
+    <t>mv_germination_fungicide_model_data_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>mv_germination_fungicide_model_2018_density_exp.rda</t>
+  </si>
+  <si>
+    <t>germination_2018_2019_density_exp.R</t>
+  </si>
+  <si>
+    <t>ev_germination_fungicide_model_2018_2019_density_exp.rda</t>
+  </si>
+  <si>
+    <t>evGermMod2</t>
+  </si>
+  <si>
+    <t>ev_germination_fungicide_model_data_2018_2019_density_exp.rda</t>
+  </si>
+  <si>
+    <t>evGermDat2</t>
+  </si>
+  <si>
+    <t>survFungD2Mod</t>
+  </si>
+  <si>
+    <t>survival_fungicide_model_2019_density_exp.rda</t>
+  </si>
+  <si>
+    <t>survD2Dat2</t>
+  </si>
+  <si>
+    <t>survival_fungicide_model_data_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>survival_2018_2019_density_exp.R</t>
   </si>
   <si>
     <t>Figure 2,
 Figure S1,
-Tables S1– S2 &amp; S7–S9,
-Results par. 1-2</t>
-  </si>
-  <si>
-    <t>Figure 3,
-Figure S2,
-Tables S10–S13 &amp; S24</t>
-  </si>
-  <si>
-    <t>Figure 4</t>
-  </si>
-  <si>
-    <t>disease_treatment_effects_2018_2019_density_exp.R</t>
-  </si>
-  <si>
-    <t>focal_severity_model_aug_2019_dens_exp.rda</t>
-  </si>
-  <si>
-    <t>sevD2Mod_sev_dens_aug</t>
-  </si>
-  <si>
-    <t>focal_severity_model_jul_2019_dens_exp.rda</t>
-  </si>
-  <si>
-    <t>sevD2Mod_sev_dens_jul</t>
-  </si>
-  <si>
-    <t>START HERE - make sure to use code in edi folder</t>
+Tables S1– S2 &amp; S7–S9</t>
+  </si>
+  <si>
+    <t>growthD2Dat2</t>
+  </si>
+  <si>
+    <t>seedD2Dat3</t>
+  </si>
+  <si>
+    <t>growthD2Mod2</t>
+  </si>
+  <si>
+    <t>focal_growth_biomass_model_2019_density_exp.rda</t>
+  </si>
+  <si>
+    <t>Figure 4,
+Tables S4, S4, S15-S16,
+S19, S23</t>
+  </si>
+  <si>
+    <t>START HERE: Fig. 5 script</t>
   </si>
 </sst>
 </file>
@@ -483,11 +650,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -496,6 +660,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,10 +688,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -815,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B32AA23-1B17-1549-AA9D-91703B674752}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -849,10 +1021,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C2" t="s">
@@ -866,8 +1038,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
       <c r="C3" t="s">
         <v>27</v>
       </c>
@@ -879,8 +1051,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
       <c r="C4" t="s">
         <v>45</v>
       </c>
@@ -892,8 +1064,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
       <c r="C5" t="s">
         <v>35</v>
       </c>
@@ -905,8 +1077,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
       <c r="C6" t="s">
         <v>37</v>
       </c>
@@ -918,8 +1090,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
       <c r="C7" t="s">
         <v>16</v>
       </c>
@@ -931,8 +1103,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
       <c r="C8" t="s">
         <v>18</v>
       </c>
@@ -944,8 +1116,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
       <c r="C9" t="s">
         <v>14</v>
       </c>
@@ -957,8 +1129,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
       <c r="C10" t="s">
         <v>15</v>
       </c>
@@ -970,8 +1142,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
       <c r="C11" t="s">
         <v>31</v>
       </c>
@@ -983,8 +1155,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
       <c r="C12" t="s">
         <v>34</v>
       </c>
@@ -996,8 +1168,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
       <c r="C13" t="s">
         <v>43</v>
       </c>
@@ -1009,8 +1181,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
       <c r="C14" t="s">
         <v>25</v>
       </c>
@@ -1022,8 +1194,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
       <c r="C15" t="s">
         <v>21</v>
       </c>
@@ -1035,8 +1207,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
       <c r="C16" t="s">
         <v>39</v>
       </c>
@@ -1048,8 +1220,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
       <c r="C17" t="s">
         <v>23</v>
       </c>
@@ -1061,10 +1233,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="A18" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C18" t="s">
@@ -1078,8 +1250,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="4"/>
       <c r="C19" t="s">
         <v>54</v>
       </c>
@@ -1091,8 +1263,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="4"/>
       <c r="C20" t="s">
         <v>56</v>
       </c>
@@ -1104,8 +1276,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="4"/>
       <c r="C21" t="s">
         <v>28</v>
       </c>
@@ -1117,8 +1289,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="4"/>
       <c r="C22" t="s">
         <v>68</v>
       </c>
@@ -1130,8 +1302,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="4"/>
       <c r="C23" t="s">
         <v>71</v>
       </c>
@@ -1142,85 +1314,289 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="2"/>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" t="s">
         <v>78</v>
       </c>
-      <c r="C24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="3"/>
-      <c r="C25" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="2"/>
+      <c r="C26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2"/>
+      <c r="C27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="2"/>
+      <c r="C28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="2"/>
+      <c r="C29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="B30" s="2"/>
+      <c r="C30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="2"/>
+      <c r="C31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="2"/>
+      <c r="C32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="2"/>
+      <c r="C33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+      <c r="B34" s="2"/>
+      <c r="C34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+      <c r="B35" s="2"/>
+      <c r="C35" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+      <c r="B36" s="2"/>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
+      <c r="B37" s="2"/>
+      <c r="C37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+      <c r="B38" s="2"/>
+      <c r="C38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" t="s">
+        <v>114</v>
+      </c>
+      <c r="E38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D25" t="s">
+      <c r="B39" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="3"/>
-      <c r="C26" t="s">
+      <c r="C39" t="s">
         <v>83</v>
       </c>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="3"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="3"/>
+      <c r="D39" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="5"/>
+      <c r="B40" s="7"/>
+      <c r="C40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="5"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="5"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="5"/>
+      <c r="B43" s="7"/>
+      <c r="C43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:E17">
     <sortCondition ref="E2:E17"/>
     <sortCondition ref="D2:D17"/>
   </sortState>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="B2:B17"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="A18:A23"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="A39:A43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
update code for repository
</commit_message>
<xml_diff>
--- a/code_data_relationships.xlsx
+++ b/code_data_relationships.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AmyKendig/Dropbox (UFL)/big-oaks-field-experiment-2018-2019/microstegium-bipolaris/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A97A12-3404-6E4B-81D7-71A438C89A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44156D79-7453-F74E-8FF5-E8E05EB5DF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42160" yWindow="500" windowWidth="26640" windowHeight="28220" xr2:uid="{A8324B94-3DCB-F445-8C87-9FFCE272213B}"/>
+    <workbookView xWindow="26460" yWindow="500" windowWidth="42220" windowHeight="28220" xr2:uid="{A8324B94-3DCB-F445-8C87-9FFCE272213B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,6 +74,208 @@
         </r>
       </text>
     </comment>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{41A46112-7B23-F346-ACAF-8AF088E75E46}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{9EC7110A-76B3-6C49-AA39-258B95460CB9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{FD68ADC4-66FE-A443-BE22-112DD293073C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">checked
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{185A5E3B-4A06-8D48-86F8-D63973504FF5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">checked
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{4294E8A9-C648-704A-8123-76BDD4EC7032}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">checked
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{A9632535-3F8B-C94C-9672-FBC1709833A1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">checked
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B18" authorId="0" shapeId="0" xr:uid="{851559DC-0FB4-1749-84B8-8125EC46E0B1}">
       <text>
         <r>
@@ -107,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E24" authorId="0" shapeId="0" xr:uid="{9BC9C5D5-31BB-B949-BDEC-529C552D763F}">
+    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{B9B1C425-8895-8646-A32A-8C0220C12E7F}">
       <text>
         <r>
           <rPr>
@@ -140,7 +342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E25" authorId="0" shapeId="0" xr:uid="{04A31C21-28D8-D047-B590-75C9051F83F3}">
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{9BC9C5D5-31BB-B949-BDEC-529C552D763F}">
       <text>
         <r>
           <rPr>
@@ -173,7 +375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E26" authorId="0" shapeId="0" xr:uid="{5EFFD713-1406-DD4F-9C99-5F013C00BA02}">
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{04A31C21-28D8-D047-B590-75C9051F83F3}">
       <text>
         <r>
           <rPr>
@@ -206,7 +408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E27" authorId="0" shapeId="0" xr:uid="{7004317B-090F-F845-9417-EE971B3D7469}">
+    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{5EFFD713-1406-DD4F-9C99-5F013C00BA02}">
       <text>
         <r>
           <rPr>
@@ -236,6 +438,241 @@
             <family val="2"/>
           </rPr>
           <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{7004317B-090F-F845-9417-EE971B3D7469}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{AB3763C7-C372-F245-9CA3-383A41EBF502}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">checked
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{4C599766-E9A7-804A-A315-720839E6D95D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">checked
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{5BD0972D-3DC1-D84D-9EDE-4D899BB4DE84}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">checked
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{6319A5F2-112D-5C49-98E2-00369D19DADA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="0" shapeId="0" xr:uid="{521CD43F-2F71-A147-8805-EF6CAFCF313A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B46" authorId="0" shapeId="0" xr:uid="{5EC2809F-E531-1C42-89CB-420AAC349D0C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">checked
+</t>
         </r>
       </text>
     </comment>
@@ -244,7 +681,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="140">
   <si>
     <t>Code</t>
   </si>
@@ -601,7 +1038,79 @@
 S19, S23</t>
   </si>
   <si>
-    <t>START HERE: Fig. 5 script</t>
+    <t>TO DO: Fig. 5 script</t>
+  </si>
+  <si>
+    <t>germ_jun</t>
+  </si>
+  <si>
+    <t>both_germination_disease_jun_2019_litter_exp.csv</t>
+  </si>
+  <si>
+    <t>litter_weight_apr_2019_litter_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_establishment_2019_litter_exp (formerly ev_germination_analysis_2019_litter_exp.R)</t>
+  </si>
+  <si>
+    <t>ev_establishment_2019_litter_exp
+(formerly ev_germination_analysis_2019_litter_exp.R)</t>
+  </si>
+  <si>
+    <t>model, data</t>
+  </si>
+  <si>
+    <t>focal_processed_growth_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>tillerD1Dat</t>
+  </si>
+  <si>
+    <t>mv_biomass_seeds_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>mvBioD2Dat</t>
+  </si>
+  <si>
+    <t>focal_growth_data_processing_2018_density_exp.R</t>
+  </si>
+  <si>
+    <t>plot_severity_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>plot_data_processing_2018_density_exp.R</t>
+  </si>
+  <si>
+    <t>plot_severity_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>plot_data_processing_2019_density_exp.R</t>
+  </si>
+  <si>
+    <t>plot_biomass_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>plotBioD2Dat</t>
+  </si>
+  <si>
+    <t>? Maybe above?</t>
+  </si>
+  <si>
+    <t>model-fitting</t>
+  </si>
+  <si>
+    <t>Directory</t>
+  </si>
+  <si>
+    <t>figures-tables</t>
+  </si>
+  <si>
+    <t>model, data,
+Table S3,
+Figure S7-S8</t>
+  </si>
+  <si>
+    <t>START WITH NEW SCRIPT</t>
   </si>
 </sst>
 </file>
@@ -650,28 +1159,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,23 +1499,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B32AA23-1B17-1549-AA9D-91703B674752}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="42.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54" customWidth="1"/>
-    <col min="5" max="5" width="53.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54" customWidth="1"/>
+    <col min="6" max="6" width="53.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1011,592 +1523,800 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="6"/>
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" t="s">
+      <c r="F3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" t="s">
         <v>45</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>46</v>
       </c>
-      <c r="E4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" t="s">
+      <c r="F4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="6"/>
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="6"/>
+      <c r="D6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="6"/>
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" t="s">
         <v>31</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="6"/>
+      <c r="D12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="6"/>
+      <c r="D13" t="s">
         <v>43</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>44</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="6"/>
+      <c r="D14" t="s">
         <v>25</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>24</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="6"/>
+      <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="6"/>
+      <c r="D16" t="s">
         <v>39</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>41</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="6"/>
+      <c r="D17" t="s">
         <v>23</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>22</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" t="s">
         <v>51</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>52</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="4"/>
-      <c r="C19" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="6"/>
+      <c r="D19" t="s">
         <v>54</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>55</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="4"/>
-      <c r="C20" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="6"/>
+      <c r="D20" t="s">
         <v>56</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>57</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="4"/>
-      <c r="C21" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="6"/>
+      <c r="D21" t="s">
         <v>28</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>11</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="4"/>
-      <c r="C22" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="6"/>
+      <c r="D22" t="s">
         <v>68</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>69</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="4"/>
-      <c r="C23" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="6"/>
+      <c r="D23" t="s">
         <v>71</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>70</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" t="s">
         <v>77</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="2"/>
-      <c r="C25" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" t="s">
         <v>79</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>78</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="2"/>
-      <c r="C26" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" t="s">
         <v>92</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>93</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="2"/>
-      <c r="C27" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" t="s">
         <v>94</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>95</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="2"/>
-      <c r="C28" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" t="s">
         <v>96</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="2"/>
-      <c r="C29" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" t="s">
         <v>97</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="2"/>
-      <c r="C30" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" t="s">
         <v>102</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="2"/>
-      <c r="C31" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" t="s">
         <v>104</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>103</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="2"/>
-      <c r="C32" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" t="s">
         <v>105</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>106</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="2"/>
-      <c r="C33" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" t="s">
         <v>107</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>108</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="2"/>
-      <c r="C34" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" t="s">
         <v>18</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>19</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="2"/>
-      <c r="C35" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" t="s">
         <v>111</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>38</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="2"/>
-      <c r="C36" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="8"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" t="s">
         <v>15</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E37" t="s">
         <v>8</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="2"/>
-      <c r="C37" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" t="s">
         <v>112</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E38" t="s">
         <v>10</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="2"/>
-      <c r="C38" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" t="s">
-        <v>114</v>
-      </c>
-      <c r="E38" t="s">
+    <row r="39" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="8"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="8"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D44" t="s">
+        <v>117</v>
+      </c>
+      <c r="E44" t="s">
+        <v>118</v>
+      </c>
+      <c r="F44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="5"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="2"/>
+      <c r="D45" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" t="s">
+        <v>119</v>
+      </c>
+      <c r="F45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" t="s">
-        <v>83</v>
-      </c>
-      <c r="D39" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="B40" s="7"/>
-      <c r="C40" t="s">
+      <c r="C46" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="7"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" t="s">
+        <v>124</v>
+      </c>
+      <c r="E47" t="s">
+        <v>123</v>
+      </c>
+      <c r="F47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="7"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" t="s">
+        <v>126</v>
+      </c>
+      <c r="E48" t="s">
+        <v>125</v>
+      </c>
+      <c r="F48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="7"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" t="s">
         <v>84</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E49" t="s">
         <v>89</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F49" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E41" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="5"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="5"/>
-      <c r="B43" s="7"/>
-      <c r="C43" t="s">
-        <v>28</v>
-      </c>
-      <c r="D43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="7"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" t="s">
+        <v>51</v>
+      </c>
+      <c r="E50" t="s">
+        <v>128</v>
+      </c>
+      <c r="F50" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="7"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E51" t="s">
+        <v>130</v>
+      </c>
+      <c r="F51" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="7"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" t="s">
+        <v>133</v>
+      </c>
+      <c r="E52" t="s">
+        <v>132</v>
+      </c>
+      <c r="F52" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:E17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:F17">
+    <sortCondition ref="F2:F17"/>
     <sortCondition ref="E2:E17"/>
-    <sortCondition ref="D2:D17"/>
   </sortState>
-  <mergeCells count="8">
+  <mergeCells count="20">
     <mergeCell ref="B2:B17"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="A18:A23"/>
+    <mergeCell ref="E41:E42"/>
     <mergeCell ref="D41:D42"/>
-    <mergeCell ref="C41:C42"/>
     <mergeCell ref="B39:B43"/>
     <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B24:B38"/>
+    <mergeCell ref="A24:A38"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="C24:C38"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="C2:C17"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="C46:C52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
update scripts for archiving
</commit_message>
<xml_diff>
--- a/code_data_relationships.xlsx
+++ b/code_data_relationships.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AmyKendig/Dropbox (UFL)/big-oaks-field-experiment-2018-2019/microstegium-bipolaris/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44156D79-7453-F74E-8FF5-E8E05EB5DF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6179FA3D-A0B0-B846-A07F-D804AB82C210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26460" yWindow="500" windowWidth="42220" windowHeight="28220" xr2:uid="{A8324B94-3DCB-F445-8C87-9FFCE272213B}"/>
+    <workbookView xWindow="33720" yWindow="500" windowWidth="34940" windowHeight="28300" xr2:uid="{A8324B94-3DCB-F445-8C87-9FFCE272213B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -276,6 +276,270 @@
         </r>
       </text>
     </comment>
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{BC69FB32-C2D6-B74B-B970-764072F01C60}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{7B19AE17-C2A5-2E49-8599-8A0149855BA5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{BABC4483-D245-E44D-B645-DC4FF91928F5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{6A71182F-9642-FB42-90EB-A10BC60C3960}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{7D6F41D4-DC5C-0F43-A61F-822E7FCBD2F7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{79EC46C4-A39E-584D-80AF-5B3DD747BF67}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{36371F02-E628-7649-811C-48BB5F5E4518}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{B989F559-1E88-D14A-85FB-0C88A86D9AEA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B18" authorId="0" shapeId="0" xr:uid="{851559DC-0FB4-1749-84B8-8125EC46E0B1}">
       <text>
         <r>
@@ -309,6 +573,171 @@
         </r>
       </text>
     </comment>
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{A2D1EFE6-80CB-5D49-BDD6-ABC7E1F3AC2E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{4E61BB64-D443-6A45-884B-EF8753EF5FD2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{F2034C8F-5B91-5140-AB0C-D939E3592E2A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{43C51EDB-7934-2348-AF7F-003D8508A836}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{9427B717-4A46-914C-B268-A48915538FC0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B24" authorId="0" shapeId="0" xr:uid="{B9B1C425-8895-8646-A32A-8C0220C12E7F}">
       <text>
         <r>
@@ -474,6 +903,204 @@
         </r>
       </text>
     </comment>
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{4697847F-E737-9948-BE91-309FFAC2CA65}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{387D7B04-5E1A-794B-8747-AD900F6470A4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{3405AB74-F8A1-304D-9811-98D3EC483ED6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{6466AC6E-044F-9B4E-9823-8F70A0222246}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{1F7E27BE-5B94-FE44-AA5C-09A0626D6EC5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{6B762316-D3B7-5D40-8964-A5BC475881F5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F34" authorId="0" shapeId="0" xr:uid="{AB3763C7-C372-F245-9CA3-383A41EBF502}">
       <text>
         <r>
@@ -576,7 +1203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{6319A5F2-112D-5C49-98E2-00369D19DADA}">
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{F92740CD-84A4-854A-8E40-50D116CE3431}">
       <text>
         <r>
           <rPr>
@@ -609,7 +1236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B44" authorId="0" shapeId="0" xr:uid="{521CD43F-2F71-A147-8805-EF6CAFCF313A}">
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{97FFCEAE-F9BB-914D-90D2-0C3CD4396E92}">
       <text>
         <r>
           <rPr>
@@ -642,7 +1269,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="B46" authorId="0" shapeId="0" xr:uid="{5EC2809F-E531-1C42-89CB-420AAC349D0C}">
+    <comment ref="B42" authorId="0" shapeId="0" xr:uid="{521CD43F-2F71-A147-8805-EF6CAFCF313A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="0" shapeId="0" xr:uid="{5EC2809F-E531-1C42-89CB-420AAC349D0C}">
       <text>
         <r>
           <rPr>
@@ -672,6 +1332,932 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">checked
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B51" authorId="0" shapeId="0" xr:uid="{BC26E8FF-4A5D-314A-A2BF-1A32CE92989D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B58" authorId="0" shapeId="0" xr:uid="{DEB9B85B-DEE9-FF49-BA45-B2EA6557D381}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B60" authorId="0" shapeId="0" xr:uid="{1A32EC44-D5C8-FE45-AFF9-000EA20F5562}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F60" authorId="0" shapeId="0" xr:uid="{2AEDE8CF-D3BF-7F4A-B982-3BC4773DEEAD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F61" authorId="0" shapeId="0" xr:uid="{A8D530E5-4374-FE43-A79C-87FC8D8168BE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E62" authorId="0" shapeId="0" xr:uid="{B8A90FAA-394C-7A49-B958-4F20226D1D09}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E63" authorId="0" shapeId="0" xr:uid="{0B27E151-B44E-E24E-ACD7-397FFA811425}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E64" authorId="0" shapeId="0" xr:uid="{13C1BB3B-AABD-4B4E-85FC-C7D79AA3D0EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E65" authorId="0" shapeId="0" xr:uid="{B841EB0E-1B59-AF4A-96A6-48B3EB8066A5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E66" authorId="0" shapeId="0" xr:uid="{C0AEA103-80E5-7442-B9AB-573AD5C8CFF7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E67" authorId="0" shapeId="0" xr:uid="{6FFBDCCD-C6CF-B044-83E9-61FCBC8ECC2E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E68" authorId="0" shapeId="0" xr:uid="{3557B35C-BF9E-9E4A-B72A-C2A3C650001B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E69" authorId="0" shapeId="0" xr:uid="{F329706E-3C3D-5543-9803-5E773C964A71}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B70" authorId="0" shapeId="0" xr:uid="{F937E24A-D3CF-F94D-A6AD-C72E3F6A9674}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F72" authorId="0" shapeId="0" xr:uid="{D0E0E3C6-4769-0942-A47A-EBA0AD189E3B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">checked
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F74" authorId="0" shapeId="0" xr:uid="{3D6506CD-ED91-394A-8438-203A18EA221B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F75" authorId="0" shapeId="0" xr:uid="{155FBAAD-B9A6-D241-A423-FD407425BC8A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F76" authorId="0" shapeId="0" xr:uid="{8F09F284-0082-7E4F-A3C2-C2A182BBB77E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F80" authorId="0" shapeId="0" xr:uid="{F425DA64-7956-D446-8044-036CDD58229F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F81" authorId="0" shapeId="0" xr:uid="{CE51600E-E4A6-F942-8A87-3027B65C90E2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B85" authorId="0" shapeId="0" xr:uid="{29353277-A920-9D4F-B293-22370C4638C1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B87" authorId="0" shapeId="0" xr:uid="{C35ED35E-4C15-EE44-A571-C55930EBF910}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B97" authorId="0" shapeId="0" xr:uid="{6A52B5EB-1C2B-3F4F-95D4-849CC30993AE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B115" authorId="0" shapeId="0" xr:uid="{B63E20E2-FB7A-7143-8EA0-F39987457B68}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B123" authorId="0" shapeId="0" xr:uid="{0209415C-36F8-8045-B54A-43C035CCB5BE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B124" authorId="0" shapeId="0" xr:uid="{C028521D-256D-BE41-9D1D-E4DE6521A2F6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B127" authorId="0" shapeId="0" xr:uid="{E36770B9-DB78-AE43-868D-E538EBE691C1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B130" authorId="0" shapeId="0" xr:uid="{83E680AF-9AA8-C843-B4AF-A40A6347757F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">left off here: ev_seeds_data_processing_2018_2019_density_exp.R
 </t>
         </r>
       </text>
@@ -681,7 +2267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="261">
   <si>
     <t>Code</t>
   </si>
@@ -755,15 +2341,9 @@
     <t>mvSeedDensMod</t>
   </si>
   <si>
-    <t>microstegium_litter_establishment_model_2018_litter_exp.rda</t>
-  </si>
-  <si>
     <t>mvEstL1Mod2</t>
   </si>
   <si>
-    <t>elymus_litter_establishment_bh_model_2019_litter_exp.rda</t>
-  </si>
-  <si>
     <t>evEstL2BhMod2</t>
   </si>
   <si>
@@ -815,13 +2395,7 @@
     <t>mvLitDat</t>
   </si>
   <si>
-    <t>microstegium_litter_establishment_data_2018_litter_exp.csv</t>
-  </si>
-  <si>
     <t>evLitDat</t>
-  </si>
-  <si>
-    <t>elymus_litter_establishment_data_2018_litter_exp.csv</t>
   </si>
   <si>
     <t>Items</t>
@@ -935,9 +2509,6 @@
 Tables S1-S2</t>
   </si>
   <si>
-    <t>bgBioD2Dat</t>
-  </si>
-  <si>
     <t>evBioD2Dat</t>
   </si>
   <si>
@@ -947,21 +2518,9 @@
     <t>ev_processed_seeds_both_year_conversion_2019_density_exp.csv</t>
   </si>
   <si>
-    <t>bg_processed_biomass_2019_density_exp.csv</t>
-  </si>
-  <si>
-    <t>bg_biomass_data_processing_2019_density_exp.R</t>
-  </si>
-  <si>
     <t>ev_biomass_seeds_oct_2019_density_exp.csv</t>
   </si>
   <si>
-    <t>ev_seeds_data_processing_2018.R</t>
-  </si>
-  <si>
-    <t>ev_seeds_data_processing_2019.R</t>
-  </si>
-  <si>
     <t>sevD2Dat3_aug2</t>
   </si>
   <si>
@@ -974,9 +2533,6 @@
     <t>ocal_severity_model_data_jul_2019_dens_exp.csv</t>
   </si>
   <si>
-    <t>mvGermD1Mod3</t>
-  </si>
-  <si>
     <t>mvGermD1Dat</t>
   </si>
   <si>
@@ -990,9 +2546,6 @@
   </si>
   <si>
     <t>ev_germination_fungicide_model_2018_2019_density_exp.rda</t>
-  </si>
-  <si>
-    <t>evGermMod2</t>
   </si>
   <si>
     <t>ev_germination_fungicide_model_data_2018_2019_density_exp.rda</t>
@@ -1033,14 +2586,6 @@
     <t>focal_growth_biomass_model_2019_density_exp.rda</t>
   </si>
   <si>
-    <t>Figure 4,
-Tables S4, S4, S15-S16,
-S19, S23</t>
-  </si>
-  <si>
-    <t>TO DO: Fig. 5 script</t>
-  </si>
-  <si>
     <t>germ_jun</t>
   </si>
   <si>
@@ -1105,12 +2650,420 @@
     <t>figures-tables</t>
   </si>
   <si>
-    <t>model, data,
+    <t>mv_processed_seeds_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>mvSeedD1Dat</t>
+  </si>
+  <si>
+    <t>mv_seeds_data_processing_2018_density_exp.R</t>
+  </si>
+  <si>
+    <t>mvSeedD2Dat</t>
+  </si>
+  <si>
+    <t>mv_plant_level_seeds_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_processed_seeds_both_year_conversion_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>evSeedD1Dat</t>
+  </si>
+  <si>
+    <t>ev_seeds_data_processing_2019.R -- combine with 2018 script</t>
+  </si>
+  <si>
+    <t>mv_seeds_data_processing_2019_density_exp.R -- combine with biomass script</t>
+  </si>
+  <si>
+    <t>survD1Dat</t>
+  </si>
+  <si>
+    <t>all_processed_survival_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>all_survival_data_processing_2018.R</t>
+  </si>
+  <si>
+    <t>Figure 4,
+Tables S4, S6, S15-S16,
+S19, S23</t>
+  </si>
+  <si>
+    <t>models, data,
 Table S3,
 Figure S7-S8</t>
   </si>
   <si>
-    <t>START WITH NEW SCRIPT</t>
+    <t>models, data, 
+Table S5</t>
+  </si>
+  <si>
+    <t>mv_litter_establishment_model_2018_litter_exp.R (formerly microstegium_litter_establishment_model_2018_litter_exp.R)</t>
+  </si>
+  <si>
+    <t>both_germination_disease_jul_2018_litter_exp.csv</t>
+  </si>
+  <si>
+    <t>estL1Dat</t>
+  </si>
+  <si>
+    <t>plotsL</t>
+  </si>
+  <si>
+    <t>plot_treatments_2018_litter_exp.csv</t>
+  </si>
+  <si>
+    <t>mv_litter_establishment_data_2018_litter_exp.csv</t>
+  </si>
+  <si>
+    <t>mv_litter_establishment_model_2018_litter_exp.rda</t>
+  </si>
+  <si>
+    <t>discrete_continuous_model_simulations.R</t>
+  </si>
+  <si>
+    <t>cont_parms</t>
+  </si>
+  <si>
+    <t>continuous_model_parameters_2018_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>discrete_model_parameters_2018_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>disc_parms</t>
+  </si>
+  <si>
+    <t>model_parameters_2018_2019_density_exp.R</t>
+  </si>
+  <si>
+    <t>continuous_AFP_model.R</t>
+  </si>
+  <si>
+    <t>continuous_AF_model.R</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>cont_AFP_mod</t>
+  </si>
+  <si>
+    <t>continuous_AP_model.R</t>
+  </si>
+  <si>
+    <t>continuous_FP_model.R</t>
+  </si>
+  <si>
+    <t>continuous_A_model.R</t>
+  </si>
+  <si>
+    <t>continuous_F_model.R</t>
+  </si>
+  <si>
+    <t>continuous_P_model.R</t>
+  </si>
+  <si>
+    <t>discrete_model.R</t>
+  </si>
+  <si>
+    <t>disc_AFP_mod</t>
+  </si>
+  <si>
+    <t>cont_AF_mod</t>
+  </si>
+  <si>
+    <t>cont_AP_mod</t>
+  </si>
+  <si>
+    <t>cont_FP_mod</t>
+  </si>
+  <si>
+    <t>cont_A_mod</t>
+  </si>
+  <si>
+    <t>cont_F_mod</t>
+  </si>
+  <si>
+    <t>cont_P_mod</t>
+  </si>
+  <si>
+    <t>Figure 5,
+Figures S9-S12</t>
+  </si>
+  <si>
+    <t>figure-prep</t>
+  </si>
+  <si>
+    <t>ev_litter_establishment_bh_model_2019_litter_exp.rda</t>
+  </si>
+  <si>
+    <t>ev_litter_establishment_data_2018_litter_exp.csv</t>
+  </si>
+  <si>
+    <t>focal_severity_model_coefficients_2019_dens_exp.csv</t>
+  </si>
+  <si>
+    <t>trans_mod_coef</t>
+  </si>
+  <si>
+    <t>evS_seeds_per_biomass_untransformed_model_2019_density_exp.rda</t>
+  </si>
+  <si>
+    <t>mv_seeds_per_biomass_untransformed_model_2019_density_exp.rda</t>
+  </si>
+  <si>
+    <t>evA_seeds_per_biomass_untransformed_model_2019_density_exp.rda</t>
+  </si>
+  <si>
+    <t>seeds_per_biomass_2018_2019_density_exp.R</t>
+  </si>
+  <si>
+    <t>mvSeedsBioD2Mod2</t>
+  </si>
+  <si>
+    <t>evSSeedsBioD2Mod2</t>
+  </si>
+  <si>
+    <t>evASeedsBioD2Mod2</t>
+  </si>
+  <si>
+    <t>ev_adult_survival_fungicide_model_2018_2019_density_exp.rda</t>
+  </si>
+  <si>
+    <t>adultSurvD1Mod2</t>
+  </si>
+  <si>
+    <t>ev_biomass_dec_2019_fungicide_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_fung_gh</t>
+  </si>
+  <si>
+    <t>litter_reu_mv_establishment_model.rda</t>
+  </si>
+  <si>
+    <t>litter_reu_establishment_analysis.R</t>
+  </si>
+  <si>
+    <t>mv_bh_mod</t>
+  </si>
+  <si>
+    <t>litter_reu_ev_establishment_model.rda</t>
+  </si>
+  <si>
+    <t>ev_bh_mod</t>
+  </si>
+  <si>
+    <t>models, data</t>
+  </si>
+  <si>
+    <t>ev_leaf_scans_jul_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>mv_leaf_scans_jul_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_leaf_scans_late_aug_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>mv_leaf_scans_late_aug_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_leaf_scans_sep_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>mv_leaf_scans_sep_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ls_ev_jul</t>
+  </si>
+  <si>
+    <t>ls_mv_jul</t>
+  </si>
+  <si>
+    <t>ls_ev_late_aug</t>
+  </si>
+  <si>
+    <t>ls_mv_late_aug</t>
+  </si>
+  <si>
+    <t>ls_ev_sep</t>
+  </si>
+  <si>
+    <t>ls_mv_sep</t>
+  </si>
+  <si>
+    <t>dt_jul</t>
+  </si>
+  <si>
+    <t>dt_late_aug</t>
+  </si>
+  <si>
+    <t>dt_sep_ev</t>
+  </si>
+  <si>
+    <t>dt_sep_mv</t>
+  </si>
+  <si>
+    <t>data-processing</t>
+  </si>
+  <si>
+    <t>ev_leaf_scans_may_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ls_ev_may</t>
+  </si>
+  <si>
+    <t>ls_mv_may</t>
+  </si>
+  <si>
+    <t>mv_leaf_scans_may_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_leaf_scans_jun_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ls_ev_jun</t>
+  </si>
+  <si>
+    <t>ls_mv_jun</t>
+  </si>
+  <si>
+    <t>mv_leaf_scans_jun_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_leaf_scans_jul_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>mv_leaf_scans_jul_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_leaf_scans_early_aug_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ls_ev_early_aug</t>
+  </si>
+  <si>
+    <t>ls_mv_early_aug</t>
+  </si>
+  <si>
+    <t>mv_leaf_scans_early_aug_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_leaf_scans_late_aug_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>mv_leaf_scans_late_aug_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_leaf_scans_sep_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>mv_leaf_scans_sep_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>dt_may</t>
+  </si>
+  <si>
+    <t>dt_jun</t>
+  </si>
+  <si>
+    <t>dt_early_aug</t>
+  </si>
+  <si>
+    <t>dt_sep</t>
+  </si>
+  <si>
+    <t>focal_disease_sep_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>soil_moisture_jun_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>soil_moisture_oct_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>canopy_cover_jul_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>plot_edge_mv_weight_jul_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>plot_edge_mv_weight_early_aug_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>plot_edge_mv_weight_late_aug_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>plot_edge_mv_weight_sep_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>sj</t>
+  </si>
+  <si>
+    <t>so</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>bj</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>bl</t>
+  </si>
+  <si>
+    <t>bs</t>
+  </si>
+  <si>
+    <t>plot_treatments_for_analyses_2018_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>temp-humidity-density-exp-20191025</t>
+  </si>
+  <si>
+    <t>dat</t>
+  </si>
+  <si>
+    <t>mvGermD1Mod2</t>
+  </si>
+  <si>
+    <t>evGermMod</t>
+  </si>
+  <si>
+    <t>models, data,
+Tables S17-S18,
+Figure S5</t>
+  </si>
+  <si>
+    <t>mv_germination_disease_set_1_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>mvGermD1Dat1</t>
+  </si>
+  <si>
+    <t>mvGermD1Dat2</t>
+  </si>
+  <si>
+    <t>mv_germination_disease_set_2_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_germination_2018_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>evGermDat</t>
+  </si>
+  <si>
+    <t>all_replacement_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>survD2Dat</t>
   </si>
 </sst>
 </file>
@@ -1159,10 +3112,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1175,15 +3140,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1499,10 +3455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B32AA23-1B17-1549-AA9D-91703B674752}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F138" sqref="F138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1517,13 +3473,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="D1" t="s">
         <v>13</v>
@@ -1532,89 +3488,89 @@
         <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>137</v>
+      <c r="A2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="6"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="3"/>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>172</v>
       </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="6"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="3"/>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>173</v>
       </c>
       <c r="F4" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="3"/>
       <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="3"/>
+      <c r="D6" t="s">
         <v>35</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>36</v>
       </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="6"/>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>38</v>
       </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="6"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="3"/>
       <c r="D7" t="s">
         <v>16</v>
       </c>
@@ -1622,13 +3578,13 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="6"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="3"/>
       <c r="D8" t="s">
         <v>18</v>
       </c>
@@ -1636,13 +3592,13 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="6"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="3"/>
       <c r="D9" t="s">
         <v>14</v>
       </c>
@@ -1650,13 +3606,13 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="3"/>
       <c r="D10" t="s">
         <v>15</v>
       </c>
@@ -1664,69 +3620,69 @@
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="3"/>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
       </c>
       <c r="F11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="3"/>
+      <c r="D12" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="6"/>
-      <c r="D12" t="s">
-        <v>34</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="6"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="3"/>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>145</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="6"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="3"/>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="6"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="3"/>
       <c r="D15" t="s">
         <v>21</v>
       </c>
@@ -1734,27 +3690,27 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="3"/>
       <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
         <v>39</v>
       </c>
-      <c r="E16" t="s">
-        <v>41</v>
-      </c>
       <c r="F16" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="3"/>
       <c r="D17" t="s">
         <v>23</v>
       </c>
@@ -1762,249 +3718,249 @@
         <v>22</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="3"/>
+      <c r="D19" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E19" t="s">
         <v>51</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="3"/>
+      <c r="D20" t="s">
         <v>52</v>
       </c>
-      <c r="F18" t="s">
+      <c r="E20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
-      <c r="D19" t="s">
+      <c r="F20" t="s">
         <v>54</v>
       </c>
-      <c r="E19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="6"/>
-      <c r="D20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="6"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="3"/>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="6"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="3"/>
       <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" t="s">
         <v>68</v>
       </c>
-      <c r="E22" t="s">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="3"/>
+      <c r="D23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" t="s">
         <v>69</v>
       </c>
-      <c r="F22" t="s">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
-      <c r="D23" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" s="6" t="s">
+      <c r="F24" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="D24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" t="s">
-        <v>76</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" t="s">
-        <v>79</v>
-      </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
       <c r="D26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" t="s">
+        <v>250</v>
+      </c>
+      <c r="E28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" t="s">
+        <v>251</v>
+      </c>
+      <c r="E30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" t="s">
         <v>92</v>
       </c>
-      <c r="E26" t="s">
-        <v>93</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" t="s">
+      <c r="F31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" t="s">
         <v>94</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E32" t="s">
         <v>95</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" t="s">
+      <c r="F32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" t="s">
         <v>96</v>
       </c>
-      <c r="E28" t="s">
-        <v>99</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" t="s">
+      <c r="E33" t="s">
         <v>97</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F33" t="s">
         <v>98</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" t="s">
-        <v>102</v>
-      </c>
-      <c r="E30" t="s">
-        <v>101</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" t="s">
-        <v>103</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" t="s">
-        <v>105</v>
-      </c>
-      <c r="E32" t="s">
-        <v>106</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" t="s">
-        <v>108</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
       <c r="D34" t="s">
         <v>18</v>
       </c>
@@ -2012,41 +3968,41 @@
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="8"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
       <c r="D35" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35" t="s">
         <v>38</v>
       </c>
-      <c r="F35" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
       <c r="D36" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E36" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
       <c r="D37" t="s">
         <v>15</v>
       </c>
@@ -2054,241 +4010,1384 @@
         <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
       <c r="D38" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="F39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="D39" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" t="s">
-        <v>87</v>
-      </c>
-      <c r="F39" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" t="s">
-        <v>84</v>
-      </c>
-      <c r="E40" t="s">
-        <v>89</v>
-      </c>
       <c r="F40" t="s">
-        <v>30</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>86</v>
+      <c r="A41" s="4"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
       </c>
       <c r="F41" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
+      <c r="A42" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" t="s">
+        <v>105</v>
+      </c>
       <c r="F42" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="8"/>
-      <c r="B43" s="6"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="6"/>
       <c r="D43" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E43" t="s">
+        <v>106</v>
+      </c>
+      <c r="F43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" t="s">
         <v>11</v>
       </c>
-      <c r="F43" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D44" t="s">
-        <v>117</v>
-      </c>
-      <c r="E44" t="s">
-        <v>118</v>
-      </c>
       <c r="F44" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="2"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
       <c r="D45" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="E45" t="s">
+        <v>110</v>
+      </c>
+      <c r="F45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="5"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" t="s">
+        <v>113</v>
+      </c>
+      <c r="E46" t="s">
+        <v>112</v>
+      </c>
+      <c r="F46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="5"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" t="s">
+        <v>82</v>
+      </c>
+      <c r="F47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="5"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" t="s">
+        <v>115</v>
+      </c>
+      <c r="F48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="5"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" t="s">
+        <v>117</v>
+      </c>
+      <c r="F49" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" t="s">
+        <v>120</v>
+      </c>
+      <c r="E50" t="s">
         <v>119</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F50" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="B46" s="6" t="s">
+      <c r="C51" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D51" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" t="s">
+        <v>126</v>
+      </c>
+      <c r="E52" t="s">
+        <v>125</v>
+      </c>
+      <c r="F52" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" t="s">
+        <v>128</v>
+      </c>
+      <c r="E53" t="s">
+        <v>129</v>
+      </c>
+      <c r="F53" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" t="s">
+        <v>131</v>
+      </c>
+      <c r="E54" t="s">
+        <v>130</v>
+      </c>
+      <c r="F54" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="4"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" t="s">
+        <v>80</v>
+      </c>
+      <c r="E55" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" t="s">
+        <v>135</v>
+      </c>
+      <c r="F56" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E57" t="s">
+        <v>110</v>
+      </c>
+      <c r="F57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58" t="s">
+        <v>142</v>
+      </c>
+      <c r="E58" t="s">
+        <v>141</v>
+      </c>
+      <c r="F58" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="5"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" t="s">
+        <v>143</v>
+      </c>
+      <c r="E59" t="s">
+        <v>144</v>
+      </c>
+      <c r="F59" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D60" t="s">
+        <v>148</v>
+      </c>
+      <c r="E60" t="s">
+        <v>149</v>
+      </c>
+      <c r="F60" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="4"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" t="s">
+        <v>151</v>
+      </c>
+      <c r="E61" t="s">
+        <v>150</v>
+      </c>
+      <c r="F61" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="4"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" t="s">
+        <v>156</v>
+      </c>
+      <c r="E62" t="s">
+        <v>153</v>
+      </c>
+      <c r="F62" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="4"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" t="s">
+        <v>164</v>
+      </c>
+      <c r="E63" t="s">
+        <v>154</v>
+      </c>
+      <c r="F63" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" t="s">
+        <v>165</v>
+      </c>
+      <c r="E64" t="s">
+        <v>157</v>
+      </c>
+      <c r="F64" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" t="s">
+        <v>166</v>
+      </c>
+      <c r="E65" t="s">
+        <v>158</v>
+      </c>
+      <c r="F65" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="4"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" t="s">
+        <v>167</v>
+      </c>
+      <c r="E66" t="s">
+        <v>159</v>
+      </c>
+      <c r="F66" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" t="s">
+        <v>168</v>
+      </c>
+      <c r="E67" t="s">
+        <v>160</v>
+      </c>
+      <c r="F67" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="4"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" t="s">
+        <v>169</v>
+      </c>
+      <c r="E68" t="s">
+        <v>161</v>
+      </c>
+      <c r="F68" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="4"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" t="s">
+        <v>163</v>
+      </c>
+      <c r="E69" t="s">
+        <v>162</v>
+      </c>
+      <c r="F69" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D70" t="s">
+        <v>113</v>
+      </c>
+      <c r="E70" t="s">
+        <v>112</v>
+      </c>
+      <c r="F70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="5"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" t="s">
+        <v>79</v>
+      </c>
+      <c r="E71" t="s">
+        <v>82</v>
+      </c>
+      <c r="F71" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="5"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" t="s">
+        <v>102</v>
+      </c>
+      <c r="E72" t="s">
+        <v>103</v>
+      </c>
+      <c r="F72" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="5"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="6" t="s">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="5"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" t="s">
+        <v>175</v>
+      </c>
+      <c r="E74" t="s">
+        <v>174</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="5"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" t="s">
+        <v>250</v>
+      </c>
+      <c r="E75" t="s">
+        <v>89</v>
+      </c>
+      <c r="F75" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="5"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" t="s">
+        <v>251</v>
+      </c>
+      <c r="E76" t="s">
+        <v>91</v>
+      </c>
+      <c r="F76" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="5"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" t="s">
+        <v>180</v>
+      </c>
+      <c r="E77" t="s">
+        <v>177</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="5"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" t="s">
+        <v>181</v>
+      </c>
+      <c r="E78" t="s">
+        <v>176</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="5"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" t="s">
+        <v>182</v>
+      </c>
+      <c r="E79" t="s">
+        <v>178</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="5"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" t="s">
+        <v>94</v>
+      </c>
+      <c r="E80" t="s">
+        <v>95</v>
+      </c>
+      <c r="F80" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="5"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" t="s">
+        <v>184</v>
+      </c>
+      <c r="E81" t="s">
+        <v>183</v>
+      </c>
+      <c r="F81" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="5"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" t="s">
+        <v>186</v>
+      </c>
+      <c r="E82" t="s">
+        <v>185</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="5"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" t="s">
+        <v>189</v>
+      </c>
+      <c r="E83" t="s">
+        <v>187</v>
+      </c>
+      <c r="F83" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="5"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" t="s">
+        <v>191</v>
+      </c>
+      <c r="E84" t="s">
+        <v>190</v>
+      </c>
+      <c r="F84" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D85" t="s">
+        <v>26</v>
+      </c>
+      <c r="E85" t="s">
+        <v>11</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="5"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" t="s">
+        <v>37</v>
+      </c>
+      <c r="E86" t="s">
+        <v>39</v>
+      </c>
+      <c r="F86" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D87" t="s">
+        <v>199</v>
+      </c>
+      <c r="E87" t="s">
+        <v>193</v>
+      </c>
+      <c r="F87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="5"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" t="s">
+        <v>200</v>
+      </c>
+      <c r="E88" t="s">
+        <v>194</v>
+      </c>
+      <c r="F88" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="5"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" t="s">
+        <v>201</v>
+      </c>
+      <c r="E89" t="s">
+        <v>195</v>
+      </c>
+      <c r="F89" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="5"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" t="s">
+        <v>202</v>
+      </c>
+      <c r="E90" t="s">
+        <v>196</v>
+      </c>
+      <c r="F90" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="5"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" t="s">
+        <v>203</v>
+      </c>
+      <c r="E91" t="s">
+        <v>197</v>
+      </c>
+      <c r="F91" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="5"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" t="s">
+        <v>204</v>
+      </c>
+      <c r="E92" t="s">
+        <v>198</v>
+      </c>
+      <c r="F92" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="5"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" t="s">
+        <v>205</v>
+      </c>
+      <c r="E93" t="s">
+        <v>55</v>
+      </c>
+      <c r="F93" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="5"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" t="s">
+        <v>206</v>
+      </c>
+      <c r="E94" t="s">
+        <v>56</v>
+      </c>
+      <c r="F94" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="5"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" t="s">
+        <v>207</v>
+      </c>
+      <c r="E95" t="s">
+        <v>57</v>
+      </c>
+      <c r="F95" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="5"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" t="s">
+        <v>208</v>
+      </c>
+      <c r="E96" t="s">
+        <v>58</v>
+      </c>
+      <c r="F96" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D97" t="s">
+        <v>211</v>
+      </c>
+      <c r="E97" t="s">
+        <v>210</v>
+      </c>
+      <c r="F97" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="5"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" t="s">
+        <v>212</v>
+      </c>
+      <c r="E98" t="s">
+        <v>213</v>
+      </c>
+      <c r="F98" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="5"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" t="s">
+        <v>215</v>
+      </c>
+      <c r="E99" t="s">
+        <v>214</v>
+      </c>
+      <c r="F99" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="5"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" t="s">
+        <v>216</v>
+      </c>
+      <c r="E100" t="s">
+        <v>217</v>
+      </c>
+      <c r="F100" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="5"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" t="s">
+        <v>199</v>
+      </c>
+      <c r="E101" t="s">
+        <v>218</v>
+      </c>
+      <c r="F101" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="5"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" t="s">
+        <v>200</v>
+      </c>
+      <c r="E102" t="s">
+        <v>219</v>
+      </c>
+      <c r="F102" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="5"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" t="s">
+        <v>221</v>
+      </c>
+      <c r="E103" t="s">
+        <v>220</v>
+      </c>
+      <c r="F103" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="5"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" t="s">
+        <v>222</v>
+      </c>
+      <c r="E104" t="s">
+        <v>223</v>
+      </c>
+      <c r="F104" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="5"/>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" t="s">
+        <v>201</v>
+      </c>
+      <c r="E105" t="s">
+        <v>224</v>
+      </c>
+      <c r="F105" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="5"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" t="s">
+        <v>202</v>
+      </c>
+      <c r="E106" t="s">
+        <v>225</v>
+      </c>
+      <c r="F106" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="5"/>
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
+      <c r="D107" t="s">
+        <v>203</v>
+      </c>
+      <c r="E107" t="s">
+        <v>226</v>
+      </c>
+      <c r="F107" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="5"/>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" t="s">
+        <v>204</v>
+      </c>
+      <c r="E108" t="s">
+        <v>227</v>
+      </c>
+      <c r="F108" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="5"/>
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
+      <c r="D109" t="s">
+        <v>228</v>
+      </c>
+      <c r="E109" t="s">
+        <v>59</v>
+      </c>
+      <c r="F109" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="5"/>
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" t="s">
+        <v>229</v>
+      </c>
+      <c r="E110" t="s">
+        <v>60</v>
+      </c>
+      <c r="F110" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="5"/>
+      <c r="B111" s="3"/>
+      <c r="C111" s="3"/>
+      <c r="D111" t="s">
+        <v>205</v>
+      </c>
+      <c r="E111" t="s">
+        <v>61</v>
+      </c>
+      <c r="F111" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="5"/>
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" t="s">
+        <v>230</v>
+      </c>
+      <c r="E112" t="s">
+        <v>62</v>
+      </c>
+      <c r="F112" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="5"/>
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+      <c r="D113" t="s">
+        <v>206</v>
+      </c>
+      <c r="E113" t="s">
+        <v>63</v>
+      </c>
+      <c r="F113" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="5"/>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" t="s">
+        <v>231</v>
+      </c>
+      <c r="E114" t="s">
+        <v>232</v>
+      </c>
+      <c r="F114" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D115" t="s">
+        <v>240</v>
+      </c>
+      <c r="E115" t="s">
+        <v>233</v>
+      </c>
+      <c r="F115" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="5"/>
+      <c r="B116" s="3"/>
+      <c r="C116" s="3"/>
+      <c r="D116" t="s">
+        <v>241</v>
+      </c>
+      <c r="E116" t="s">
+        <v>234</v>
+      </c>
+      <c r="F116" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="5"/>
+      <c r="B117" s="3"/>
+      <c r="C117" s="3"/>
+      <c r="D117" t="s">
+        <v>242</v>
+      </c>
+      <c r="E117" t="s">
+        <v>235</v>
+      </c>
+      <c r="F117" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="5"/>
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
+      <c r="D118" t="s">
+        <v>243</v>
+      </c>
+      <c r="E118" t="s">
+        <v>236</v>
+      </c>
+      <c r="F118" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="5"/>
+      <c r="B119" s="3"/>
+      <c r="C119" s="3"/>
+      <c r="D119" t="s">
+        <v>244</v>
+      </c>
+      <c r="E119" t="s">
+        <v>237</v>
+      </c>
+      <c r="F119" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="5"/>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+      <c r="D120" t="s">
+        <v>245</v>
+      </c>
+      <c r="E120" t="s">
+        <v>238</v>
+      </c>
+      <c r="F120" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="5"/>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" t="s">
+        <v>246</v>
+      </c>
+      <c r="E121" t="s">
+        <v>239</v>
+      </c>
+      <c r="F121" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="5"/>
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
+      <c r="D122" t="s">
+        <v>26</v>
+      </c>
+      <c r="E122" t="s">
+        <v>247</v>
+      </c>
+      <c r="F122" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B123" t="s">
+        <v>69</v>
+      </c>
+      <c r="C123" t="s">
+        <v>209</v>
+      </c>
+      <c r="D123" t="s">
+        <v>249</v>
+      </c>
+      <c r="E123" t="s">
+        <v>248</v>
+      </c>
+      <c r="F123" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D124" t="s">
+        <v>254</v>
+      </c>
+      <c r="E124" t="s">
+        <v>253</v>
+      </c>
+      <c r="F124" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="4"/>
+      <c r="B125" s="3"/>
+      <c r="C125" s="3"/>
+      <c r="D125" t="s">
+        <v>255</v>
+      </c>
+      <c r="E125" t="s">
+        <v>256</v>
+      </c>
+      <c r="F125" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="4"/>
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+      <c r="D126" t="s">
+        <v>258</v>
+      </c>
+      <c r="E126" t="s">
+        <v>257</v>
+      </c>
+      <c r="F126" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D127" t="s">
+        <v>134</v>
+      </c>
+      <c r="E127" t="s">
         <v>135</v>
       </c>
-      <c r="D46" t="s">
-        <v>28</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="F127" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="5"/>
+      <c r="B128" s="3"/>
+      <c r="C128" s="3"/>
+      <c r="D128" t="s">
+        <v>260</v>
+      </c>
+      <c r="E128" t="s">
+        <v>259</v>
+      </c>
+      <c r="F128" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="5"/>
+      <c r="B129" s="3"/>
+      <c r="C129" s="3"/>
+      <c r="D129" t="s">
+        <v>26</v>
+      </c>
+      <c r="E129" t="s">
         <v>11</v>
       </c>
-      <c r="F46" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="7"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" t="s">
-        <v>124</v>
-      </c>
-      <c r="E47" t="s">
-        <v>123</v>
-      </c>
-      <c r="F47" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" t="s">
-        <v>126</v>
-      </c>
-      <c r="E48" t="s">
-        <v>125</v>
-      </c>
-      <c r="F48" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="7"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" t="s">
-        <v>84</v>
-      </c>
-      <c r="E49" t="s">
-        <v>89</v>
-      </c>
-      <c r="F49" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" t="s">
-        <v>51</v>
-      </c>
-      <c r="E50" t="s">
-        <v>128</v>
-      </c>
-      <c r="F50" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="7"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" t="s">
-        <v>54</v>
-      </c>
-      <c r="E51" t="s">
-        <v>130</v>
-      </c>
-      <c r="F51" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" t="s">
-        <v>133</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="F129" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B130" t="s">
         <v>132</v>
-      </c>
-      <c r="F52" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2296,27 +5395,55 @@
     <sortCondition ref="F2:F17"/>
     <sortCondition ref="E2:E17"/>
   </sortState>
-  <mergeCells count="20">
+  <mergeCells count="48">
+    <mergeCell ref="C97:C114"/>
+    <mergeCell ref="B97:B114"/>
+    <mergeCell ref="A97:A114"/>
+    <mergeCell ref="C115:C122"/>
+    <mergeCell ref="B115:B122"/>
+    <mergeCell ref="A115:A122"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="C87:C96"/>
+    <mergeCell ref="B87:B96"/>
+    <mergeCell ref="A87:A96"/>
+    <mergeCell ref="B51:B57"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="C24:C38"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C2:C17"/>
+    <mergeCell ref="C51:C57"/>
     <mergeCell ref="B2:B17"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="A18:A23"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="A39:A43"/>
     <mergeCell ref="B24:B38"/>
     <mergeCell ref="A24:A38"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="C24:C38"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="C2:C17"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="C46:C52"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="C44:C50"/>
+    <mergeCell ref="C70:C84"/>
+    <mergeCell ref="B70:B84"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="C60:C69"/>
+    <mergeCell ref="B60:B69"/>
+    <mergeCell ref="A60:A69"/>
+    <mergeCell ref="C124:C126"/>
+    <mergeCell ref="B124:B126"/>
+    <mergeCell ref="A124:A126"/>
+    <mergeCell ref="C127:C129"/>
+    <mergeCell ref="B127:B129"/>
+    <mergeCell ref="A127:A129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2338,30 +5465,30 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -2394,90 +5521,90 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
format scripts for archiving
</commit_message>
<xml_diff>
--- a/code_data_relationships.xlsx
+++ b/code_data_relationships.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AmyKendig/Dropbox (UFL)/big-oaks-field-experiment-2018-2019/microstegium-bipolaris/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6179FA3D-A0B0-B846-A07F-D804AB82C210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16F697E-71DC-5C4F-B50D-21B208A44723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="500" windowWidth="34940" windowHeight="28300" xr2:uid="{A8324B94-3DCB-F445-8C87-9FFCE272213B}"/>
+    <workbookView xWindow="33700" yWindow="500" windowWidth="34940" windowHeight="28300" xr2:uid="{A8324B94-3DCB-F445-8C87-9FFCE272213B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1269,6 +1269,39 @@
         </r>
       </text>
     </comment>
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{8C2BDEC4-C665-F240-93ED-1040B81D75C1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B42" authorId="0" shapeId="0" xr:uid="{521CD43F-2F71-A147-8805-EF6CAFCF313A}">
       <text>
         <r>
@@ -1336,6 +1369,39 @@
         </r>
       </text>
     </comment>
+    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{330B5F0B-25E6-E649-99C0-5CF8885AA28F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B51" authorId="0" shapeId="0" xr:uid="{BC26E8FF-4A5D-314A-A2BF-1A32CE92989D}">
       <text>
         <r>
@@ -1369,6 +1435,204 @@
         </r>
       </text>
     </comment>
+    <comment ref="F52" authorId="0" shapeId="0" xr:uid="{6AB02879-6B9F-E040-9FC8-42A684EDA483}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F53" authorId="0" shapeId="0" xr:uid="{4595E04D-EE1A-8A4E-A74E-7DDB11EF891D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F54" authorId="0" shapeId="0" xr:uid="{A186365E-AE82-1341-9E66-3E1E6EA06457}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F55" authorId="0" shapeId="0" xr:uid="{C6E49E42-D042-E24C-B795-B0A5F86FBF29}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F56" authorId="0" shapeId="0" xr:uid="{C3608049-23B8-E84D-B42A-8340BA04FD9F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F57" authorId="0" shapeId="0" xr:uid="{AF51B2FC-F79C-FA4B-822A-809BFC8917A8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B58" authorId="0" shapeId="0" xr:uid="{DEB9B85B-DEE9-FF49-BA45-B2EA6557D381}">
       <text>
         <r>
@@ -1832,6 +2096,39 @@
         </r>
       </text>
     </comment>
+    <comment ref="F73" authorId="0" shapeId="0" xr:uid="{2BD75879-D212-EB4D-9677-E963539E865F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F74" authorId="0" shapeId="0" xr:uid="{3D6506CD-ED91-394A-8438-203A18EA221B}">
       <text>
         <r>
@@ -1931,6 +2228,105 @@
         </r>
       </text>
     </comment>
+    <comment ref="F77" authorId="0" shapeId="0" xr:uid="{3D0718B6-B4D4-454A-95A1-CD34D13E9DF0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F78" authorId="0" shapeId="0" xr:uid="{B55FE495-07A3-244B-AA20-170670ED0BA4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F79" authorId="0" shapeId="0" xr:uid="{2D1128EB-47A9-D74A-A8BA-D02DAF1EB5E9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F80" authorId="0" shapeId="0" xr:uid="{F425DA64-7956-D446-8044-036CDD58229F}">
       <text>
         <r>
@@ -1997,6 +2393,72 @@
         </r>
       </text>
     </comment>
+    <comment ref="F83" authorId="0" shapeId="0" xr:uid="{59E4940E-5DC9-D64C-9B00-4FDD1BC1DD23}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F84" authorId="0" shapeId="0" xr:uid="{21B8EE43-6BB4-6244-97B0-B76D15CA9070}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B85" authorId="0" shapeId="0" xr:uid="{29353277-A920-9D4F-B293-22370C4638C1}">
       <text>
         <r>
@@ -2228,6 +2690,39 @@
         </r>
       </text>
     </comment>
+    <comment ref="F127" authorId="0" shapeId="0" xr:uid="{F466A29D-4834-7947-9459-17E182AEBC67}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B130" authorId="0" shapeId="0" xr:uid="{83E680AF-9AA8-C843-B4AF-A40A6347757F}">
       <text>
         <r>
@@ -2257,7 +2752,339 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">left off here: ev_seeds_data_processing_2018_2019_density_exp.R
+          <t xml:space="preserve">checked
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B144" authorId="0" shapeId="0" xr:uid="{125A43CE-EA7C-9E46-B0D5-3E7BB223348B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B146" authorId="0" shapeId="0" xr:uid="{5D85CFB8-59E2-894C-826A-D7A1187CA722}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B148" authorId="0" shapeId="0" xr:uid="{D3FACA40-21C2-0A45-8E90-EE3799B29A2C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E151" authorId="0" shapeId="0" xr:uid="{CF789057-6098-744C-84E3-99F3F30FA63E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>original version in intermediate-data becaues it was manually edited to add seed counts. I didn't think this made sense for archived version. Removed uncounted rows for data folder.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B152" authorId="0" shapeId="0" xr:uid="{81CA8206-2DA9-6545-A12B-E3391D1ABF50}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F154" authorId="0" shapeId="0" xr:uid="{A510380E-77DF-F743-A4B4-4098695C43E9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F155" authorId="0" shapeId="0" xr:uid="{1BE802EE-EDD4-FB4C-A587-67C04FFABB91}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">checked
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B156" authorId="0" shapeId="0" xr:uid="{62874D6B-7BAE-6043-8DBC-E6F98E367535}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B158" authorId="0" shapeId="0" xr:uid="{99C86498-DFB9-3E4B-96AF-8A79DA5D0868}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>checked</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F158" authorId="0" shapeId="0" xr:uid="{17324DDE-5F4F-EA4F-93F5-EEF5B0E84635}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Kendig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">checked
 </t>
         </r>
       </text>
@@ -2267,7 +3094,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="307">
   <si>
     <t>Code</t>
   </si>
@@ -2656,9 +3483,6 @@
     <t>mvSeedD1Dat</t>
   </si>
   <si>
-    <t>mv_seeds_data_processing_2018_density_exp.R</t>
-  </si>
-  <si>
     <t>mvSeedD2Dat</t>
   </si>
   <si>
@@ -2671,19 +3495,10 @@
     <t>evSeedD1Dat</t>
   </si>
   <si>
-    <t>ev_seeds_data_processing_2019.R -- combine with 2018 script</t>
-  </si>
-  <si>
-    <t>mv_seeds_data_processing_2019_density_exp.R -- combine with biomass script</t>
-  </si>
-  <si>
     <t>survD1Dat</t>
   </si>
   <si>
     <t>all_processed_survival_2018_density_exp.csv</t>
-  </si>
-  <si>
-    <t>all_survival_data_processing_2018.R</t>
   </si>
   <si>
     <t>Figure 4,
@@ -3064,6 +3879,156 @@
   </si>
   <si>
     <t>survD2Dat</t>
+  </si>
+  <si>
+    <t>ev_seeds_data_processing_2018_2019_density_exp.R -- previously ev_seeds_data_processing_2018.R and _2019.R</t>
+  </si>
+  <si>
+    <t>ev_spikelets_2018_density_litter_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_seed_subset_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_seeds_early_aug_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_seeds_2018_litter_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_spikelets_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ev_seed_subset_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>di</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>dea</t>
+  </si>
+  <si>
+    <t>dla</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>spikelets</t>
+  </si>
+  <si>
+    <t>biomass</t>
+  </si>
+  <si>
+    <t>seeds</t>
+  </si>
+  <si>
+    <t>plants_jun</t>
+  </si>
+  <si>
+    <t>plants_jul</t>
+  </si>
+  <si>
+    <t>plants_eau</t>
+  </si>
+  <si>
+    <t>plants_lau</t>
+  </si>
+  <si>
+    <t>plants_sep</t>
+  </si>
+  <si>
+    <t>fjn</t>
+  </si>
+  <si>
+    <t>focal_size_disease_jun_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>fjl</t>
+  </si>
+  <si>
+    <t>mv_seeds_biomass_data_processing_2018_density_exp.R -- previously mv_seeds_data_processing_2018_density_exp.R</t>
+  </si>
+  <si>
+    <t>bag</t>
+  </si>
+  <si>
+    <t>mv_bag_seed_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>bio</t>
+  </si>
+  <si>
+    <t>mv_biomass_oct_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>bio_seeds</t>
+  </si>
+  <si>
+    <t>mv_seeds_data_processing_2019_density_exp.R</t>
+  </si>
+  <si>
+    <t>bag_seeds</t>
+  </si>
+  <si>
+    <t>mv_bag_seeds_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>bag_notes</t>
+  </si>
+  <si>
+    <t>mv_biomass_seeds_counted_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>bio_seeds_conv</t>
+  </si>
+  <si>
+    <t>models</t>
+  </si>
+  <si>
+    <t>MvEstDat</t>
+  </si>
+  <si>
+    <t>litter_reu_mv_establishment_data.csv</t>
+  </si>
+  <si>
+    <t>EvEstDat</t>
+  </si>
+  <si>
+    <t>litter_reu_ev_establishment_data.csv</t>
+  </si>
+  <si>
+    <t>fea</t>
+  </si>
+  <si>
+    <t>focal_status_early_aug_2018_density_exp.csv</t>
+  </si>
+  <si>
+    <t>ala</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>ew</t>
+  </si>
+  <si>
+    <t>ev_winter_survival_apr_2019_density_exp.csv</t>
+  </si>
+  <si>
+    <t>all_survival_data_processing_2018_density_exp.R -- previously all_survival_data_processing_2018.R</t>
+  </si>
+  <si>
+    <t>eseeds</t>
+  </si>
+  <si>
+    <t>data-processing-tier2</t>
   </si>
 </sst>
 </file>
@@ -3124,10 +4089,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3156,6 +4121,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3455,10 +4424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B32AA23-1B17-1549-AA9D-91703B674752}">
-  <dimension ref="A1:F130"/>
+  <dimension ref="A1:F171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F138" sqref="F138"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158:B165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3492,10 +4461,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -3512,36 +4481,36 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" t="s">
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="3"/>
       <c r="D4" t="s">
         <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F4" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="3"/>
       <c r="D5" t="s">
         <v>33</v>
@@ -3554,8 +4523,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="3"/>
       <c r="D6" t="s">
         <v>35</v>
@@ -3568,8 +4537,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="3"/>
       <c r="D7" t="s">
         <v>16</v>
@@ -3582,8 +4551,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="3"/>
       <c r="D8" t="s">
         <v>18</v>
@@ -3596,8 +4565,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="3"/>
       <c r="D9" t="s">
         <v>14</v>
@@ -3610,8 +4579,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="3"/>
       <c r="D10" t="s">
         <v>15</v>
@@ -3624,8 +4593,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="3"/>
       <c r="D11" t="s">
         <v>29</v>
@@ -3638,8 +4607,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="3"/>
       <c r="D12" t="s">
         <v>32</v>
@@ -3652,36 +4621,36 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="3"/>
       <c r="D13" t="s">
         <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F13" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="3"/>
       <c r="D14" t="s">
         <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="3"/>
       <c r="D15" t="s">
         <v>21</v>
@@ -3694,8 +4663,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="3"/>
       <c r="D16" t="s">
         <v>37</v>
@@ -3708,8 +4677,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="3"/>
       <c r="D17" t="s">
         <v>23</v>
@@ -3722,10 +4691,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -3742,8 +4711,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="3"/>
       <c r="D19" t="s">
         <v>50</v>
@@ -3756,8 +4725,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="3"/>
       <c r="D20" t="s">
         <v>52</v>
@@ -3770,8 +4739,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="4"/>
       <c r="C21" s="3"/>
       <c r="D21" t="s">
         <v>26</v>
@@ -3784,8 +4753,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="3"/>
       <c r="D22" t="s">
         <v>64</v>
@@ -3798,8 +4767,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" t="s">
         <v>67</v>
@@ -3812,8 +4781,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>137</v>
+      <c r="A24" s="5" t="s">
+        <v>133</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>71</v>
@@ -3832,7 +4801,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
+      <c r="A25" s="5"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" t="s">
@@ -3846,7 +4815,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
+      <c r="A26" s="5"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" t="s">
@@ -3860,7 +4829,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
+      <c r="A27" s="5"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" t="s">
@@ -3874,11 +4843,11 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
+      <c r="A28" s="5"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E28" t="s">
         <v>89</v>
@@ -3888,7 +4857,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
+      <c r="A29" s="5"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" t="s">
@@ -3902,11 +4871,11 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
+      <c r="A30" s="5"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E30" t="s">
         <v>91</v>
@@ -3916,7 +4885,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
+      <c r="A31" s="5"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" t="s">
@@ -3930,7 +4899,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
+      <c r="A32" s="5"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" t="s">
@@ -3944,7 +4913,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
+      <c r="A33" s="5"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" t="s">
@@ -3958,7 +4927,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
+      <c r="A34" s="5"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" t="s">
@@ -3972,7 +4941,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
+      <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" t="s">
@@ -3986,7 +4955,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
+      <c r="A36" s="5"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" t="s">
@@ -4000,7 +4969,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
+      <c r="A37" s="5"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" t="s">
@@ -4014,7 +4983,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
+      <c r="A38" s="5"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" t="s">
@@ -4028,7 +4997,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -4048,7 +5017,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
+      <c r="A40" s="5"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" t="s">
@@ -4058,11 +5027,11 @@
         <v>81</v>
       </c>
       <c r="F40" t="s">
-        <v>132</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
+      <c r="A41" s="5"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" t="s">
@@ -4110,8 +5079,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>138</v>
+      <c r="A44" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>38</v>
@@ -4130,7 +5099,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="5"/>
+      <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" t="s">
@@ -4144,7 +5113,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="5"/>
+      <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" t="s">
@@ -4158,7 +5127,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="5"/>
+      <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" t="s">
@@ -4172,7 +5141,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="5"/>
+      <c r="A48" s="4"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" t="s">
@@ -4186,7 +5155,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="5"/>
+      <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" t="s">
@@ -4200,7 +5169,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="5"/>
+      <c r="A50" s="4"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" t="s">
@@ -4214,8 +5183,8 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
-        <v>139</v>
+      <c r="A51" s="5" t="s">
+        <v>135</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>30</v>
@@ -4234,7 +5203,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="4"/>
+      <c r="A52" s="5"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" t="s">
@@ -4244,39 +5213,39 @@
         <v>125</v>
       </c>
       <c r="F52" t="s">
-        <v>127</v>
+        <v>280</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="4"/>
+      <c r="A53" s="5"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" t="s">
+        <v>127</v>
+      </c>
+      <c r="E53" t="s">
         <v>128</v>
       </c>
-      <c r="E53" t="s">
-        <v>129</v>
-      </c>
       <c r="F53" t="s">
-        <v>133</v>
+        <v>286</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="4"/>
+      <c r="A54" s="5"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F54" t="s">
-        <v>132</v>
+        <v>257</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="4"/>
+      <c r="A55" s="5"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" t="s">
@@ -4286,25 +5255,25 @@
         <v>81</v>
       </c>
       <c r="F55" t="s">
-        <v>132</v>
+        <v>257</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="4"/>
+      <c r="A56" s="5"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E56" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F56" t="s">
-        <v>136</v>
+        <v>304</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="4"/>
+      <c r="A57" s="5"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" t="s">
@@ -4318,194 +5287,194 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>122</v>
       </c>
       <c r="D58" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E58" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F58" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="5"/>
+      <c r="A59" s="4"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" t="s">
+        <v>139</v>
+      </c>
+      <c r="E59" t="s">
+        <v>140</v>
+      </c>
+      <c r="F59" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="E59" t="s">
-        <v>144</v>
-      </c>
-      <c r="F59" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>124</v>
       </c>
       <c r="D60" t="s">
+        <v>144</v>
+      </c>
+      <c r="E60" t="s">
+        <v>145</v>
+      </c>
+      <c r="F60" t="s">
         <v>148</v>
       </c>
-      <c r="E60" t="s">
-        <v>149</v>
-      </c>
-      <c r="F60" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="4"/>
+      <c r="A61" s="5"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E61" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F61" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="4"/>
+      <c r="A62" s="5"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E62" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F62" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="4"/>
+      <c r="A63" s="5"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E63" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F63" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="4"/>
+      <c r="A64" s="5"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E64" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F64" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="4"/>
+      <c r="A65" s="5"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E65" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F65" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="4"/>
+      <c r="A66" s="5"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E66" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F66" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="4"/>
+      <c r="A67" s="5"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E67" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F67" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="4"/>
+      <c r="A68" s="5"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E68" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F68" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="4"/>
+      <c r="A69" s="5"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E69" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F69" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D70" t="s">
         <v>113</v>
@@ -4518,7 +5487,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="5"/>
+      <c r="A71" s="4"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" t="s">
@@ -4532,7 +5501,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="5"/>
+      <c r="A72" s="4"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" t="s">
@@ -4546,7 +5515,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="5"/>
+      <c r="A73" s="4"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" t="s">
@@ -4560,25 +5529,25 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="5"/>
+      <c r="A74" s="4"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E74" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="5"/>
+      <c r="A75" s="4"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E75" t="s">
         <v>89</v>
@@ -4588,11 +5557,11 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="5"/>
+      <c r="A76" s="4"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E76" t="s">
         <v>91</v>
@@ -4602,49 +5571,49 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="5"/>
+      <c r="A77" s="4"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E77" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="5"/>
+      <c r="A78" s="4"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E78" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="5"/>
+      <c r="A79" s="4"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E79" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="5"/>
+      <c r="A80" s="4"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" t="s">
@@ -4658,64 +5627,64 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="5"/>
+      <c r="A81" s="4"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E81" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F81" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="5"/>
+      <c r="A82" s="4"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E82" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="5"/>
+      <c r="A83" s="4"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E83" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F83" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="5"/>
+      <c r="A84" s="4"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E84" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F84" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>40</v>
@@ -4734,7 +5703,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="5"/>
+      <c r="A86" s="4"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" t="s">
@@ -4748,101 +5717,101 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D87" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E87" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F87" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="5"/>
+      <c r="A88" s="4"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E88" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F88" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="5"/>
+      <c r="A89" s="4"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E89" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F89" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="5"/>
+      <c r="A90" s="4"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E90" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F90" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="5"/>
+      <c r="A91" s="4"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E91" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F91" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="5"/>
+      <c r="A92" s="4"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E92" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F92" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="5"/>
+      <c r="A93" s="4"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E93" t="s">
         <v>55</v>
@@ -4852,11 +5821,11 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="5"/>
+      <c r="A94" s="4"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E94" t="s">
         <v>56</v>
@@ -4866,11 +5835,11 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="5"/>
+      <c r="A95" s="4"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E95" t="s">
         <v>57</v>
@@ -4880,11 +5849,11 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="5"/>
+      <c r="A96" s="4"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E96" t="s">
         <v>58</v>
@@ -4894,185 +5863,185 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D97" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E97" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F97" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="5"/>
+      <c r="A98" s="4"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E98" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F98" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="5"/>
+      <c r="A99" s="4"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E99" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F99" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="5"/>
+      <c r="A100" s="4"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E100" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F100" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="5"/>
+      <c r="A101" s="4"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E101" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F101" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="5"/>
+      <c r="A102" s="4"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E102" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F102" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="5"/>
+      <c r="A103" s="4"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E103" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F103" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" s="5"/>
+      <c r="A104" s="4"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E104" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F104" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="5"/>
+      <c r="A105" s="4"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E105" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F105" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="5"/>
+      <c r="A106" s="4"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E106" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F106" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" s="5"/>
+      <c r="A107" s="4"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E107" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F107" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="5"/>
+      <c r="A108" s="4"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E108" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F108" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109" s="5"/>
+      <c r="A109" s="4"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E109" t="s">
         <v>59</v>
@@ -5082,11 +6051,11 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110" s="5"/>
+      <c r="A110" s="4"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E110" t="s">
         <v>60</v>
@@ -5096,11 +6065,11 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" s="5"/>
+      <c r="A111" s="4"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E111" t="s">
         <v>61</v>
@@ -5110,11 +6079,11 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112" s="5"/>
+      <c r="A112" s="4"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E112" t="s">
         <v>62</v>
@@ -5124,11 +6093,11 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" s="5"/>
+      <c r="A113" s="4"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E113" t="s">
         <v>63</v>
@@ -5138,132 +6107,132 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A114" s="5"/>
+      <c r="A114" s="4"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
       <c r="D114" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E114" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F114" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A115" s="5" t="s">
+      <c r="A115" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D115" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E115" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F115" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A116" s="5"/>
+      <c r="A116" s="4"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
       <c r="D116" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E116" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F116" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" s="5"/>
+      <c r="A117" s="4"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E117" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F117" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" s="5"/>
+      <c r="A118" s="4"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
       <c r="D118" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E118" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F118" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119" s="5"/>
+      <c r="A119" s="4"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
       <c r="D119" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E119" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F119" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A120" s="5"/>
+      <c r="A120" s="4"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
       <c r="D120" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E120" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F120" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" s="5"/>
+      <c r="A121" s="4"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
       <c r="D121" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E121" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F121" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A122" s="5"/>
+      <c r="A122" s="4"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" t="s">
         <v>26</v>
       </c>
       <c r="E122" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F122" t="s">
         <v>28</v>
@@ -5277,21 +6246,21 @@
         <v>69</v>
       </c>
       <c r="C123" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D123" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E123" t="s">
+        <v>244</v>
+      </c>
+      <c r="F123" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="F123" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124" s="4" t="s">
-        <v>252</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>90</v>
@@ -5300,46 +6269,46 @@
         <v>122</v>
       </c>
       <c r="D124" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E124" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F124" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A125" s="4"/>
+      <c r="A125" s="5"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E125" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F125" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A126" s="4"/>
+      <c r="A126" s="5"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E126" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F126" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A127" s="5" t="s">
-        <v>192</v>
+      <c r="A127" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>98</v>
@@ -5348,31 +6317,31 @@
         <v>122</v>
       </c>
       <c r="D127" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E127" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F127" t="s">
-        <v>136</v>
+        <v>304</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A128" s="5"/>
+      <c r="A128" s="4"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E128" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F128" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129" s="5"/>
+      <c r="A129" s="4"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" t="s">
@@ -5386,16 +6355,593 @@
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B130" t="s">
-        <v>132</v>
-      </c>
+      <c r="A130" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D130" t="s">
+        <v>264</v>
+      </c>
+      <c r="E130" t="s">
+        <v>258</v>
+      </c>
+      <c r="F130" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="4"/>
+      <c r="B131" s="3"/>
+      <c r="C131" s="3"/>
+      <c r="D131" t="s">
+        <v>265</v>
+      </c>
+      <c r="E131" t="s">
+        <v>259</v>
+      </c>
+      <c r="F131" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="4"/>
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+      <c r="D132" t="s">
+        <v>266</v>
+      </c>
+      <c r="E132" t="s">
+        <v>260</v>
+      </c>
+      <c r="F132" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="4"/>
+      <c r="B133" s="3"/>
+      <c r="C133" s="3"/>
+      <c r="D133" t="s">
+        <v>267</v>
+      </c>
+      <c r="E133" t="s">
+        <v>56</v>
+      </c>
+      <c r="F133" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="4"/>
+      <c r="B134" s="3"/>
+      <c r="C134" s="3"/>
+      <c r="D134" t="s">
+        <v>268</v>
+      </c>
+      <c r="E134" t="s">
+        <v>57</v>
+      </c>
+      <c r="F134" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="4"/>
+      <c r="B135" s="3"/>
+      <c r="C135" s="3"/>
+      <c r="D135" t="s">
+        <v>267</v>
+      </c>
+      <c r="E135" t="s">
+        <v>261</v>
+      </c>
+      <c r="F135" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="4"/>
+      <c r="B136" s="3"/>
+      <c r="C136" s="3"/>
+      <c r="D136" t="s">
+        <v>269</v>
+      </c>
+      <c r="E136" t="s">
+        <v>262</v>
+      </c>
+      <c r="F136" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="4"/>
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" t="s">
+        <v>270</v>
+      </c>
+      <c r="E137" t="s">
+        <v>82</v>
+      </c>
+      <c r="F137" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" s="4"/>
+      <c r="B138" s="3"/>
+      <c r="C138" s="3"/>
+      <c r="D138" t="s">
+        <v>271</v>
+      </c>
+      <c r="E138" t="s">
+        <v>263</v>
+      </c>
+      <c r="F138" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" s="4"/>
+      <c r="B139" s="3"/>
+      <c r="C139" s="3"/>
+      <c r="D139" t="s">
+        <v>272</v>
+      </c>
+      <c r="E139" t="s">
+        <v>60</v>
+      </c>
+      <c r="F139" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="4"/>
+      <c r="B140" s="3"/>
+      <c r="C140" s="3"/>
+      <c r="D140" t="s">
+        <v>273</v>
+      </c>
+      <c r="E140" t="s">
+        <v>61</v>
+      </c>
+      <c r="F140" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="4"/>
+      <c r="B141" s="3"/>
+      <c r="C141" s="3"/>
+      <c r="D141" t="s">
+        <v>274</v>
+      </c>
+      <c r="E141" t="s">
+        <v>62</v>
+      </c>
+      <c r="F141" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="4"/>
+      <c r="B142" s="3"/>
+      <c r="C142" s="3"/>
+      <c r="D142" t="s">
+        <v>275</v>
+      </c>
+      <c r="E142" t="s">
+        <v>63</v>
+      </c>
+      <c r="F142" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" s="4"/>
+      <c r="B143" s="3"/>
+      <c r="C143" s="3"/>
+      <c r="D143" t="s">
+        <v>276</v>
+      </c>
+      <c r="E143" t="s">
+        <v>228</v>
+      </c>
+      <c r="F143" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D144" t="s">
+        <v>277</v>
+      </c>
+      <c r="E144" t="s">
+        <v>278</v>
+      </c>
+      <c r="F144" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" s="4"/>
+      <c r="B145" s="3"/>
+      <c r="C145" s="3"/>
+      <c r="D145" t="s">
+        <v>279</v>
+      </c>
+      <c r="E145" t="s">
+        <v>55</v>
+      </c>
+      <c r="F145" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D146" t="s">
+        <v>281</v>
+      </c>
+      <c r="E146" t="s">
+        <v>282</v>
+      </c>
+      <c r="F146" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" s="4"/>
+      <c r="B147" s="3"/>
+      <c r="C147" s="3"/>
+      <c r="D147" t="s">
+        <v>283</v>
+      </c>
+      <c r="E147" t="s">
+        <v>284</v>
+      </c>
+      <c r="F147" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D148" t="s">
+        <v>285</v>
+      </c>
+      <c r="E148" t="s">
+        <v>112</v>
+      </c>
+      <c r="F148" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" s="4"/>
+      <c r="B149" s="3"/>
+      <c r="C149" s="3"/>
+      <c r="D149" t="s">
+        <v>287</v>
+      </c>
+      <c r="E149" t="s">
+        <v>288</v>
+      </c>
+      <c r="F149" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" s="4"/>
+      <c r="B150" s="3"/>
+      <c r="C150" s="3"/>
+      <c r="D150" t="s">
+        <v>289</v>
+      </c>
+      <c r="E150" t="s">
+        <v>228</v>
+      </c>
+      <c r="F150" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" s="4"/>
+      <c r="B151" s="3"/>
+      <c r="C151" s="3"/>
+      <c r="D151" t="s">
+        <v>291</v>
+      </c>
+      <c r="E151" t="s">
+        <v>290</v>
+      </c>
+      <c r="F151" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A152" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D152" t="s">
+        <v>113</v>
+      </c>
+      <c r="E152" t="s">
+        <v>112</v>
+      </c>
+      <c r="F152" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A153" s="4"/>
+      <c r="B153" s="3"/>
+      <c r="C153" s="3"/>
+      <c r="D153" t="s">
+        <v>79</v>
+      </c>
+      <c r="E153" t="s">
+        <v>82</v>
+      </c>
+      <c r="F153" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" s="4"/>
+      <c r="B154" s="3"/>
+      <c r="C154" s="3"/>
+      <c r="D154" t="s">
+        <v>127</v>
+      </c>
+      <c r="E154" t="s">
+        <v>128</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A155" s="4"/>
+      <c r="B155" s="3"/>
+      <c r="C155" s="3"/>
+      <c r="D155" t="s">
+        <v>80</v>
+      </c>
+      <c r="E155" t="s">
+        <v>81</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D156" t="s">
+        <v>293</v>
+      </c>
+      <c r="E156" t="s">
+        <v>294</v>
+      </c>
+      <c r="F156" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A157" s="4"/>
+      <c r="B157" s="3"/>
+      <c r="C157" s="3"/>
+      <c r="D157" t="s">
+        <v>295</v>
+      </c>
+      <c r="E157" t="s">
+        <v>296</v>
+      </c>
+      <c r="F157" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D158" t="s">
+        <v>305</v>
+      </c>
+      <c r="E158" t="s">
+        <v>129</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" s="4"/>
+      <c r="B159" s="3"/>
+      <c r="C159" s="3"/>
+      <c r="D159" t="s">
+        <v>277</v>
+      </c>
+      <c r="E159" t="s">
+        <v>278</v>
+      </c>
+      <c r="F159" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" s="4"/>
+      <c r="B160" s="3"/>
+      <c r="C160" s="3"/>
+      <c r="D160" t="s">
+        <v>279</v>
+      </c>
+      <c r="E160" t="s">
+        <v>55</v>
+      </c>
+      <c r="F160" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A161" s="4"/>
+      <c r="B161" s="3"/>
+      <c r="C161" s="3"/>
+      <c r="D161" t="s">
+        <v>297</v>
+      </c>
+      <c r="E161" t="s">
+        <v>298</v>
+      </c>
+      <c r="F161" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" s="4"/>
+      <c r="B162" s="3"/>
+      <c r="C162" s="3"/>
+      <c r="D162" t="s">
+        <v>299</v>
+      </c>
+      <c r="E162" t="s">
+        <v>56</v>
+      </c>
+      <c r="F162" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163" s="4"/>
+      <c r="B163" s="3"/>
+      <c r="C163" s="3"/>
+      <c r="D163" t="s">
+        <v>300</v>
+      </c>
+      <c r="E163" t="s">
+        <v>57</v>
+      </c>
+      <c r="F163" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A164" s="4"/>
+      <c r="B164" s="3"/>
+      <c r="C164" s="3"/>
+      <c r="D164" t="s">
+        <v>301</v>
+      </c>
+      <c r="E164" t="s">
+        <v>58</v>
+      </c>
+      <c r="F164" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A165" s="4"/>
+      <c r="B165" s="3"/>
+      <c r="C165" s="3"/>
+      <c r="D165" t="s">
+        <v>302</v>
+      </c>
+      <c r="E165" t="s">
+        <v>303</v>
+      </c>
+      <c r="F165" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F166" s="1"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F167" s="1"/>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F168" s="1"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F169" s="1"/>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F170" s="1"/>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F171" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:F17">
     <sortCondition ref="F2:F17"/>
     <sortCondition ref="E2:E17"/>
   </sortState>
-  <mergeCells count="48">
+  <mergeCells count="69">
+    <mergeCell ref="C158:C165"/>
+    <mergeCell ref="B158:B165"/>
+    <mergeCell ref="A158:A165"/>
+    <mergeCell ref="C152:C155"/>
+    <mergeCell ref="B152:B155"/>
+    <mergeCell ref="A152:A155"/>
+    <mergeCell ref="C156:C157"/>
+    <mergeCell ref="B156:B157"/>
+    <mergeCell ref="A156:A157"/>
+    <mergeCell ref="C148:C151"/>
+    <mergeCell ref="B148:B151"/>
+    <mergeCell ref="A148:A151"/>
+    <mergeCell ref="C144:C145"/>
+    <mergeCell ref="B144:B145"/>
+    <mergeCell ref="A144:A145"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="B146:B147"/>
+    <mergeCell ref="A146:A147"/>
     <mergeCell ref="C97:C114"/>
     <mergeCell ref="B97:B114"/>
     <mergeCell ref="A97:A114"/>
@@ -5408,8 +6954,6 @@
     <mergeCell ref="C87:C96"/>
     <mergeCell ref="B87:B96"/>
     <mergeCell ref="A87:A96"/>
-    <mergeCell ref="B51:B57"/>
-    <mergeCell ref="A51:A57"/>
     <mergeCell ref="C24:C38"/>
     <mergeCell ref="C18:C23"/>
     <mergeCell ref="A39:A41"/>
@@ -5429,6 +6973,8 @@
     <mergeCell ref="B44:B50"/>
     <mergeCell ref="A44:A50"/>
     <mergeCell ref="C44:C50"/>
+    <mergeCell ref="B51:B57"/>
+    <mergeCell ref="A51:A57"/>
     <mergeCell ref="C70:C84"/>
     <mergeCell ref="B70:B84"/>
     <mergeCell ref="A70:A84"/>
@@ -5438,6 +6984,9 @@
     <mergeCell ref="C60:C69"/>
     <mergeCell ref="B60:B69"/>
     <mergeCell ref="A60:A69"/>
+    <mergeCell ref="C130:C143"/>
+    <mergeCell ref="B130:B143"/>
+    <mergeCell ref="A130:A143"/>
     <mergeCell ref="C124:C126"/>
     <mergeCell ref="B124:B126"/>
     <mergeCell ref="A124:A126"/>

</xml_diff>